<commit_message>
Update baru - akun facebook dan lokasi target.xlsx
</commit_message>
<xml_diff>
--- a/baru - akun facebook dan lokasi target.xlsx
+++ b/baru - akun facebook dan lokasi target.xlsx
@@ -965,6 +965,9 @@
       <c r="C1">
         <v>41</v>
       </c>
+      <c r="D1">
+        <v>41</v>
+      </c>
       <c r="E1">
         <v>20</v>
       </c>
@@ -996,6 +999,9 @@
       <c r="C3">
         <v>43</v>
       </c>
+      <c r="D3">
+        <v>43</v>
+      </c>
       <c r="E3">
         <v>20</v>
       </c>
@@ -1010,8 +1016,11 @@
       <c r="C4">
         <v>103</v>
       </c>
+      <c r="D4">
+        <v>40</v>
+      </c>
       <c r="E4">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1024,6 +1033,9 @@
       <c r="C5">
         <v>24</v>
       </c>
+      <c r="D5">
+        <v>24</v>
+      </c>
       <c r="E5">
         <v>24</v>
       </c>
@@ -1038,6 +1050,9 @@
       <c r="C6">
         <v>45</v>
       </c>
+      <c r="D6">
+        <v>45</v>
+      </c>
       <c r="E6">
         <v>20</v>
       </c>
@@ -1052,6 +1067,9 @@
       <c r="C7">
         <v>32</v>
       </c>
+      <c r="D7">
+        <v>32</v>
+      </c>
       <c r="E7">
         <v>15</v>
       </c>
@@ -1066,6 +1084,9 @@
       <c r="C8" s="1">
         <v>54</v>
       </c>
+      <c r="D8">
+        <v>54</v>
+      </c>
       <c r="E8">
         <v>27</v>
       </c>
@@ -1080,6 +1101,9 @@
       <c r="C9">
         <v>33</v>
       </c>
+      <c r="D9">
+        <v>33</v>
+      </c>
       <c r="E9">
         <v>15</v>
       </c>
@@ -1094,6 +1118,9 @@
       <c r="C10">
         <v>31</v>
       </c>
+      <c r="D10">
+        <v>31</v>
+      </c>
       <c r="E10">
         <v>15</v>
       </c>
@@ -1159,6 +1186,9 @@
       <c r="C14">
         <v>37</v>
       </c>
+      <c r="D14">
+        <v>37</v>
+      </c>
       <c r="E14">
         <v>15</v>
       </c>
@@ -1173,6 +1203,9 @@
       <c r="C15">
         <v>37</v>
       </c>
+      <c r="D15">
+        <v>37</v>
+      </c>
       <c r="E15">
         <v>15</v>
       </c>
@@ -1187,6 +1220,9 @@
       <c r="C16">
         <v>30</v>
       </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
       <c r="E16">
         <v>15</v>
       </c>
@@ -1201,6 +1237,9 @@
       <c r="C17">
         <v>37</v>
       </c>
+      <c r="D17">
+        <v>37</v>
+      </c>
       <c r="E17">
         <v>15</v>
       </c>
@@ -1213,6 +1252,9 @@
         <v>33</v>
       </c>
       <c r="C18">
+        <v>39</v>
+      </c>
+      <c r="D18">
         <v>39</v>
       </c>
       <c r="E18">

</xml_diff>